<commit_message>
updated for Oct 29 data
</commit_message>
<xml_diff>
--- a/output/natl_grandtots_bothyears_6daysout.xlsx
+++ b/output/natl_grandtots_bothyears_6daysout.xlsx
@@ -384,13 +384,13 @@
         <v>33416590</v>
       </c>
       <c r="B2">
-        <v>64148234</v>
+        <v>68966658</v>
       </c>
       <c r="C2">
-        <v>30731644</v>
+        <v>35550068</v>
       </c>
       <c r="D2">
-        <v>91.97</v>
+        <v>106.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>